<commit_message>
edit fxml file 19.10.2021 16:56(доделать)
</commit_message>
<xml_diff>
--- a/src/main/resources/template/Export.xlsx
+++ b/src/main/resources/template/Export.xlsx
@@ -515,7 +515,7 @@
   <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="160" zoomScaleNormal="166" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -551,57 +551,57 @@
       <c r="A4" s="9"/>
       <c r="B4" s="9"/>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="8" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
     </row>
-    <row r="6" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="12"/>
     </row>
-    <row r="7" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
       <c r="B7" s="4"/>
     </row>
-    <row r="8" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
       <c r="B8" s="6"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3"/>
       <c r="B9" s="13"/>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
       <c r="B10" s="14"/>
       <c r="D10" s="2"/>
     </row>
-    <row r="11" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3"/>
       <c r="B11" s="15"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
     </row>
-    <row r="13" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
     </row>
-    <row r="14" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:4" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" spans="1:1" s="8" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" spans="1:1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" spans="1:1" ht="10.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:4" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" spans="1:1" s="8" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" spans="1:1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:1" ht="9.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
     </row>
-    <row r="20" spans="1:1" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:1" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" spans="1:1" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" spans="1:1" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" spans="1:1" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" spans="1:1" s="2" customFormat="1" ht="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:1" s="2" customFormat="1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="24" spans="1:1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="25" spans="1:1" ht="10.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>